<commit_message>
chore: replace company-specific management group IDs with placeholder
Replaced all instances of the company-specific management group ID
(e1f3e196-aa55-4709-9c55-0e334c0b444f) with a placeholder value
(11111111111111111111111111111111111111111) to make this repository
suitable for use as a template.

Changed across 13 files:
- Policy assignments (custom, NIST, comprehensive, MCSB, STIG)
- Policy set definitions
- Policy exemptions
- Global settings
- CI/CD configuration files (.gitlab-ci.yml, GitHub workflows)
- Documentation (GITLAB-QUICKSTART.md, GITLAB-SETUP.md, SWITCHING-TO-ENFORCEMENT.md)

This change makes the repository portable and ready for others to use
by replacing tenant-specific identifiers with generic placeholders.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Azure_CC_Local_Controls.xlsx
+++ b/Azure_CC_Local_Controls.xlsx
@@ -6,11 +6,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="EPAC Coverage Summary3" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="EPAC Coverage Summary2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="EPAC Coverage Summary1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="EPAC Coverage Summary" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Local Controls" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="EPAC Coverage Summary4" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="EPAC Coverage Summary3" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="EPAC Coverage Summary2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="EPAC Coverage Summary1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="EPAC Coverage Summary" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Local Controls" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
@@ -464,7 +465,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-11-13 12:14:17</t>
+          <t>2025-11-13 12:56:16</t>
         </is>
       </c>
     </row>
@@ -639,7 +640,7 @@
     <row r="21">
       <c r="A21" s="7" t="inlineStr">
         <is>
-          <t>Quick Wins (Custom Policies)</t>
+          <t>Custom Control Family Policies</t>
         </is>
       </c>
       <c r="B21" s="7" t="inlineStr"/>
@@ -647,7 +648,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>• Mandatory Tags: Owner, CostCenter, Environment, DataClassification, CriticalityLevel</t>
+          <t>• CM Family - Mandatory Tags: Owner, CostCenter, Environment, DataClassification, CriticalityLevel</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -655,7 +656,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>• Backup Enforcement: Azure Backup required on all VMs and SQL databases</t>
+          <t>• CP Family - Backup Enforcement: Azure Backup required on all VMs and SQL databases</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -663,7 +664,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>• Geo-Redundancy: Require GRS/GZRS storage, multi-region for critical apps</t>
+          <t>• CP Family - Geo-Redundancy: Require GRS/GZRS storage, multi-region for critical apps</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -671,7 +672,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>• DDoS Protection: Require Standard tier on public-facing resources</t>
+          <t>• SC Family - DDoS Protection: Require Standard tier on public-facing resources</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -679,7 +680,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>• Update Management: Require enrollment on all compute resources</t>
+          <t>• SI Family - Update Management: Require enrollment on all compute resources</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -687,7 +688,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>• Resource Locks: Require locks on production resource groups</t>
+          <t>• CM Family - Resource Locks: Require locks on production resource groups</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -695,7 +696,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>• WAF Enforcement: Require Application Gateway WAF on public web apps</t>
+          <t>• SI Family - WAF Enforcement: Require Application Gateway WAF on public web apps</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -769,7 +770,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-11-13 12:13:44</t>
+          <t>2025-11-13 12:14:17</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1272,7 +1273,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-11-13 12:13:26</t>
+          <t>2025-11-13 12:13:44</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1761,7 +1762,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-11-13 12:08:30</t>
+          <t>2025-11-13 12:13:26</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -2187,6 +2188,495 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="35" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="6" max="6"/>
+    <col width="35" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>EPAC &amp; MDC Coverage Analysis</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr"/>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>Managed by EPAC</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>MDC Coverage</t>
+        </is>
+      </c>
+      <c r="E1" s="10" t="inlineStr">
+        <is>
+          <t>Implementation Details</t>
+        </is>
+      </c>
+      <c r="F1" s="10" t="inlineStr">
+        <is>
+          <t>Custom Policy Opportunity</t>
+        </is>
+      </c>
+      <c r="G1" s="10" t="inlineStr">
+        <is>
+          <t>Priority/Action</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Generated:</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-11-13 12:08:30</t>
+        </is>
+      </c>
+      <c r="C2" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="6" customHeight="1"/>
+    <row r="5" ht="6" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>Overall Statistics</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr"/>
+      <c r="C5" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="6" customHeight="1"/>
+    <row r="7" ht="6" customHeight="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Total Controls Analyzed:</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>71</v>
+      </c>
+      <c r="C7" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="6" customHeight="1"/>
+    <row r="9" ht="6" customHeight="1">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Fully Covered (YES):</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>30 (42.3%)</t>
+        </is>
+      </c>
+      <c r="C9" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="6" customHeight="1"/>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Partially Covered (PARTIAL):</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1 (1.4%)</t>
+        </is>
+      </c>
+      <c r="C11" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="6" customHeight="1"/>
+    <row r="13" ht="6" customHeight="1">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Not Covered (NO):</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>40 (56.3%)</t>
+        </is>
+      </c>
+      <c r="C13" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="6" customHeight="1">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Overall Coverage Score:</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>43.0%</t>
+        </is>
+      </c>
+      <c r="C15" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="6" customHeight="1"/>
+    <row r="17" ht="6" customHeight="1"/>
+    <row r="18" ht="6" customHeight="1">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>Custom Policy Opportunities</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="inlineStr"/>
+      <c r="C18" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="6" customHeight="1"/>
+    <row r="20" ht="6" customHeight="1">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Controls with Custom Policy Opportunities:</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>24</v>
+      </c>
+      <c r="C20" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="6" customHeight="1"/>
+    <row r="23" ht="6" customHeight="1">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>Priority Actions</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="inlineStr"/>
+      <c r="C23" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="6" customHeight="1"/>
+    <row r="25" ht="6" customHeight="1">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>1. CP-9: CREATE BACKUP ENFORCEMENT POLICY</t>
+        </is>
+      </c>
+      <c r="B25" s="8" t="inlineStr">
+        <is>
+          <t>CRITICAL - Require Azure Backup on all VMs/DBs</t>
+        </is>
+      </c>
+      <c r="C25" s="12" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D25" s="13" t="inlineStr">
+        <is>
+          <t>YES - MDC recommends Azure Backup</t>
+        </is>
+      </c>
+      <c r="E25" s="13" t="inlineStr">
+        <is>
+          <t>Customer responsibility - Configure Azure Backup</t>
+        </is>
+      </c>
+      <c r="F25" s="16" t="inlineStr">
+        <is>
+          <t>CREATE POLICY TO ENFORCE AZURE BACKUP ON ALL VMs AND DATABASES - HIGH PRIORITY!</t>
+        </is>
+      </c>
+      <c r="G25" s="17" t="inlineStr">
+        <is>
+          <t>CRITICAL - CUSTOM BACKUP POLICY REQUIRED</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="6" customHeight="1"/>
+    <row r="27" ht="6" customHeight="1">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2. CP Controls: Document DR/BCP procedures</t>
+        </is>
+      </c>
+      <c r="B27" s="8" t="inlineStr">
+        <is>
+          <t>CRITICAL - 0% coverage for contingency planning</t>
+        </is>
+      </c>
+      <c r="C27" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="6" customHeight="1"/>
+    <row r="29" ht="6" customHeight="1">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>3. CM-8/CM-12: Enforce mandatory tagging</t>
+        </is>
+      </c>
+      <c r="B29" s="9" t="inlineStr">
+        <is>
+          <t>HIGH - Data classification, criticality, owner tags</t>
+        </is>
+      </c>
+      <c r="C29" s="15" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="D29" s="13" t="inlineStr">
+        <is>
+          <t>YES - MDC provides asset inventory</t>
+        </is>
+      </c>
+      <c r="E29" s="13" t="inlineStr">
+        <is>
+          <t>Azure Resource Graph provides complete inventory, MDC asset inventory dashboard</t>
+        </is>
+      </c>
+      <c r="F29" s="13" t="inlineStr">
+        <is>
+          <t>Create policy to enforce mandatory tags (Owner, CostCenter, Environment, DataClassification)</t>
+        </is>
+      </c>
+      <c r="G29" s="13" t="inlineStr">
+        <is>
+          <t>IMPLEMENTED - CUSTOM TAG POLICY RECOMMENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>4. SC-5: Enforce DDoS Protection</t>
+        </is>
+      </c>
+      <c r="B31" s="9" t="inlineStr">
+        <is>
+          <t>HIGH - Require on public IPs/VNETs</t>
+        </is>
+      </c>
+      <c r="C31" s="15" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="D31" s="13" t="inlineStr">
+        <is>
+          <t>YES - MDC recommends DDoS Protection</t>
+        </is>
+      </c>
+      <c r="E31" s="13" t="inlineStr">
+        <is>
+          <t>Azure DDoS Protection Standard, Application Gateway WAF</t>
+        </is>
+      </c>
+      <c r="F31" s="13" t="inlineStr">
+        <is>
+          <t>Create policy to require DDoS Protection on public IPs/VNETs</t>
+        </is>
+      </c>
+      <c r="G31" s="13" t="inlineStr">
+        <is>
+          <t>IMPLEMENTED - CUSTOM ENFORCEMENT RECOMMENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>5. SI-2(2): Enforce Update Management</t>
+        </is>
+      </c>
+      <c r="B33" s="9" t="inlineStr">
+        <is>
+          <t>HIGH - All VMs must enroll</t>
+        </is>
+      </c>
+      <c r="C33" s="15" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="D33" s="13" t="inlineStr">
+        <is>
+          <t>YES - MDC Defender for Endpoint tracks patching</t>
+        </is>
+      </c>
+      <c r="E33" s="13" t="inlineStr">
+        <is>
+          <t>Azure Update Management, MDC vulnerability scanner</t>
+        </is>
+      </c>
+      <c r="F33" s="13" t="inlineStr">
+        <is>
+          <t>Create policy to enforce update management enrollment on all VMs</t>
+        </is>
+      </c>
+      <c r="G33" s="13" t="inlineStr">
+        <is>
+          <t>IMPLEMENTED - CUSTOM ENFORCEMENT RECOMMENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="7" t="inlineStr">
+        <is>
+          <t>Quick Wins (Custom Policies)</t>
+        </is>
+      </c>
+      <c r="B36" s="7" t="inlineStr"/>
+      <c r="C36" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>• Mandatory Tags: Owner, CostCenter, Environment, DataClassification, CriticalityLevel</t>
+        </is>
+      </c>
+      <c r="C38" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>• Backup Enforcement: Azure Backup required on all VMs and SQL databases</t>
+        </is>
+      </c>
+      <c r="C40" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>• Geo-Redundancy: Require GRS/GZRS storage, multi-region for critical apps</t>
+        </is>
+      </c>
+      <c r="C42" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>• DDoS Protection: Require Standard tier on public-facing resources</t>
+        </is>
+      </c>
+      <c r="C44" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>• Update Management: Require enrollment on all compute resources</t>
+        </is>
+      </c>
+      <c r="C46" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>• Resource Locks: Require locks on production resource groups</t>
+        </is>
+      </c>
+      <c r="C48" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>• WAF Enforcement: Require Application Gateway WAF on public web apps</t>
+        </is>
+      </c>
+      <c r="C50" s="11" t="inlineStr">
+        <is>
+          <t>NOT MAPPED</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>